<commit_message>
removed pom.xml and added lib folder
</commit_message>
<xml_diff>
--- a/Resources/Dose Response/Information.xlsx
+++ b/Resources/Dose Response/Information.xlsx
@@ -5,16 +5,14 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larz\Desktop\dose_response_pics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Larz\Desktop\Thesis\Resources\Dose Response\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="13650"/>
+    <workbookView xWindow="0" yWindow="150" windowWidth="20100" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725" iterateDelta="0"/>
 </workbook>
@@ -133,102 +131,6 @@
     <t>Eye malformation (no eyes, smaller, less pigmentation)</t>
   </si>
   <si>
-    <t>image101.png</t>
-  </si>
-  <si>
-    <t>image103.png</t>
-  </si>
-  <si>
-    <t>image105.png</t>
-  </si>
-  <si>
-    <t>image107.png</t>
-  </si>
-  <si>
-    <t>image109.png</t>
-  </si>
-  <si>
-    <t>image111.png</t>
-  </si>
-  <si>
-    <t>image113.png</t>
-  </si>
-  <si>
-    <t>image115.png</t>
-  </si>
-  <si>
-    <t>image117.png</t>
-  </si>
-  <si>
-    <t>image119.png</t>
-  </si>
-  <si>
-    <t>image121.png</t>
-  </si>
-  <si>
-    <t>image123.png</t>
-  </si>
-  <si>
-    <t>image125.png</t>
-  </si>
-  <si>
-    <t>image127.png</t>
-  </si>
-  <si>
-    <t>image131.png</t>
-  </si>
-  <si>
-    <t>image133.png</t>
-  </si>
-  <si>
-    <t>image135.png</t>
-  </si>
-  <si>
-    <t>image137.png</t>
-  </si>
-  <si>
-    <t>image141.png</t>
-  </si>
-  <si>
-    <t>image143.png</t>
-  </si>
-  <si>
-    <t>image145.png</t>
-  </si>
-  <si>
-    <t>image147.png</t>
-  </si>
-  <si>
-    <t>image149.png</t>
-  </si>
-  <si>
-    <t>image151.png</t>
-  </si>
-  <si>
-    <t>image153.png</t>
-  </si>
-  <si>
-    <t>image157.png</t>
-  </si>
-  <si>
-    <t>image159.png</t>
-  </si>
-  <si>
-    <t>image163.png</t>
-  </si>
-  <si>
-    <t>image165.png</t>
-  </si>
-  <si>
-    <t>image167.png</t>
-  </si>
-  <si>
-    <t>image169.png</t>
-  </si>
-  <si>
-    <t>image171.png</t>
-  </si>
-  <si>
     <t>image005.png</t>
   </si>
   <si>
@@ -346,46 +248,142 @@
     <t>image083.png</t>
   </si>
   <si>
-    <t>image085.png</t>
-  </si>
-  <si>
-    <t>image087.png</t>
-  </si>
-  <si>
-    <t>image089.png</t>
-  </si>
-  <si>
-    <t>image091.png</t>
-  </si>
-  <si>
-    <t>image093.png</t>
-  </si>
-  <si>
-    <t>image095.png</t>
-  </si>
-  <si>
-    <t>image097.png</t>
-  </si>
-  <si>
-    <t>image099.png</t>
-  </si>
-  <si>
     <t>image073.png</t>
   </si>
   <si>
-    <t>image129.png</t>
-  </si>
-  <si>
-    <t>image139.png</t>
-  </si>
-  <si>
-    <t>image155.png</t>
-  </si>
-  <si>
-    <t>image161.png</t>
-  </si>
-  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>image001.png</t>
+  </si>
+  <si>
+    <t>image002.png</t>
+  </si>
+  <si>
+    <t>image003.png</t>
+  </si>
+  <si>
+    <t>image004.png</t>
+  </si>
+  <si>
+    <t>image006.png</t>
+  </si>
+  <si>
+    <t>image008.png</t>
+  </si>
+  <si>
+    <t>image010.png</t>
+  </si>
+  <si>
+    <t>image012.png</t>
+  </si>
+  <si>
+    <t>image014.png</t>
+  </si>
+  <si>
+    <t>image016.png</t>
+  </si>
+  <si>
+    <t>image018.png</t>
+  </si>
+  <si>
+    <t>image020.png</t>
+  </si>
+  <si>
+    <t>image022.png</t>
+  </si>
+  <si>
+    <t>image024.png</t>
+  </si>
+  <si>
+    <t>image026.png</t>
+  </si>
+  <si>
+    <t>image028.png</t>
+  </si>
+  <si>
+    <t>image030.png</t>
+  </si>
+  <si>
+    <t>image032.png</t>
+  </si>
+  <si>
+    <t>image034.png</t>
+  </si>
+  <si>
+    <t>image036.png</t>
+  </si>
+  <si>
+    <t>image038.png</t>
+  </si>
+  <si>
+    <t>image040.png</t>
+  </si>
+  <si>
+    <t>image042.png</t>
+  </si>
+  <si>
+    <t>image044.png</t>
+  </si>
+  <si>
+    <t>image046.png</t>
+  </si>
+  <si>
+    <t>image048.png</t>
+  </si>
+  <si>
+    <t>image050.png</t>
+  </si>
+  <si>
+    <t>image052.png</t>
+  </si>
+  <si>
+    <t>image054.png</t>
+  </si>
+  <si>
+    <t>image056.png</t>
+  </si>
+  <si>
+    <t>image058.png</t>
+  </si>
+  <si>
+    <t>image060.png</t>
+  </si>
+  <si>
+    <t>image062.png</t>
+  </si>
+  <si>
+    <t>image064.png</t>
+  </si>
+  <si>
+    <t>image066.png</t>
+  </si>
+  <si>
+    <t>image068.png</t>
+  </si>
+  <si>
+    <t>image070.png</t>
+  </si>
+  <si>
+    <t>image072.png</t>
+  </si>
+  <si>
+    <t>image074.png</t>
+  </si>
+  <si>
+    <t>image076.png</t>
+  </si>
+  <si>
+    <t>image078.png</t>
+  </si>
+  <si>
+    <t>image080.png</t>
+  </si>
+  <si>
+    <t>image082.png</t>
+  </si>
+  <si>
+    <t>image084.png</t>
   </si>
 </sst>
 </file>
@@ -823,7 +821,7 @@
   <dimension ref="A1:M86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -925,10 +923,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>18</v>
@@ -966,10 +964,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>18</v>
@@ -1007,10 +1005,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>18</v>
@@ -1048,10 +1046,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>77</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>18</v>
@@ -1089,10 +1087,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>18</v>
@@ -1130,10 +1128,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>78</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>18</v>
@@ -1171,10 +1169,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>18</v>
@@ -1212,10 +1210,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>18</v>
@@ -1253,10 +1251,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="1" t="s">
         <v>73</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>18</v>
@@ -1294,10 +1292,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>18</v>
@@ -1335,10 +1333,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>36</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>18</v>
@@ -1376,10 +1374,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>81</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
@@ -1416,11 +1414,11 @@
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>77</v>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -1457,11 +1455,11 @@
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>78</v>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -1498,11 +1496,11 @@
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>79</v>
+      <c r="B17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>12</v>
@@ -1539,11 +1537,11 @@
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>80</v>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>83</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
@@ -1580,11 +1578,11 @@
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>81</v>
+      <c r="B19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
@@ -1621,11 +1619,11 @@
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>82</v>
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -1662,11 +1660,11 @@
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>83</v>
+      <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
@@ -1703,11 +1701,11 @@
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>84</v>
+      <c r="B22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>12</v>
@@ -1744,11 +1742,11 @@
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>85</v>
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
@@ -1785,10 +1783,10 @@
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>86</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -1826,11 +1824,11 @@
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>87</v>
+      <c r="B25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>42</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>12</v>
@@ -1867,11 +1865,11 @@
       <c r="A26" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>88</v>
+      <c r="B26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>12</v>
@@ -1911,8 +1909,8 @@
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>89</v>
+      <c r="C27" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>18</v>
@@ -1952,8 +1950,8 @@
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>90</v>
+      <c r="C28" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>18</v>
@@ -1993,8 +1991,8 @@
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>91</v>
+      <c r="C29" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>18</v>
@@ -2034,8 +2032,8 @@
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>92</v>
+      <c r="C30" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>18</v>
@@ -2075,8 +2073,8 @@
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>93</v>
+      <c r="C31" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>18</v>
@@ -2116,8 +2114,8 @@
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>94</v>
+      <c r="C32" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>18</v>
@@ -2157,8 +2155,8 @@
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>95</v>
+      <c r="C33" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>18</v>
@@ -2198,8 +2196,8 @@
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>96</v>
+      <c r="C34" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>18</v>
@@ -2239,8 +2237,8 @@
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>97</v>
+      <c r="C35" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>18</v>
@@ -2280,8 +2278,8 @@
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>98</v>
+      <c r="C36" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
@@ -2321,8 +2319,8 @@
       <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>112</v>
+      <c r="C37" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>18</v>
@@ -2362,8 +2360,8 @@
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>99</v>
+      <c r="C38" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>18</v>
@@ -2403,8 +2401,8 @@
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>100</v>
+      <c r="C39" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>18</v>
@@ -2444,8 +2442,8 @@
       <c r="B40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>101</v>
+      <c r="C40" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>18</v>
@@ -2485,8 +2483,8 @@
       <c r="B41" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>102</v>
+      <c r="C41" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>18</v>
@@ -2526,8 +2524,8 @@
       <c r="B42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>103</v>
+      <c r="C42" s="9" t="s">
+        <v>95</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>18</v>
@@ -2567,8 +2565,8 @@
       <c r="B43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>104</v>
+      <c r="C43" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>18</v>
@@ -2608,8 +2606,8 @@
       <c r="B44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>105</v>
+      <c r="C44" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>18</v>
@@ -2649,8 +2647,8 @@
       <c r="B45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>106</v>
+      <c r="C45" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>18</v>
@@ -2690,8 +2688,8 @@
       <c r="B46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>107</v>
+      <c r="C46" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>18</v>
@@ -2731,8 +2729,8 @@
       <c r="B47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>108</v>
+      <c r="C47" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>18</v>
@@ -2772,8 +2770,8 @@
       <c r="B48" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>109</v>
+      <c r="C48" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>18</v>
@@ -2813,8 +2811,8 @@
       <c r="B49" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>110</v>
+      <c r="C49" s="9" t="s">
+        <v>54</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>18</v>
@@ -2854,8 +2852,8 @@
       <c r="B50" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>111</v>
+      <c r="C50" s="9" t="s">
+        <v>99</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>18</v>
@@ -2895,8 +2893,8 @@
       <c r="B51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>33</v>
+      <c r="C51" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>18</v>
@@ -2936,8 +2934,8 @@
       <c r="B52" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>34</v>
+      <c r="C52" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>18</v>
@@ -2977,8 +2975,8 @@
       <c r="B53" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>35</v>
+      <c r="C53" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>18</v>
@@ -3018,8 +3016,8 @@
       <c r="B54" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>36</v>
+      <c r="C54" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>18</v>
@@ -3059,8 +3057,8 @@
       <c r="B55" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>37</v>
+      <c r="C55" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>18</v>
@@ -3100,8 +3098,8 @@
       <c r="B56" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>38</v>
+      <c r="C56" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>18</v>
@@ -3141,8 +3139,8 @@
       <c r="B57" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>39</v>
+      <c r="C57" s="9" t="s">
+        <v>58</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>18</v>
@@ -3182,8 +3180,8 @@
       <c r="B58" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>40</v>
+      <c r="C58" s="9" t="s">
+        <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>18</v>
@@ -3223,8 +3221,8 @@
       <c r="B59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>41</v>
+      <c r="C59" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>18</v>
@@ -3264,8 +3262,8 @@
       <c r="B60" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>42</v>
+      <c r="C60" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>12</v>
@@ -3305,8 +3303,8 @@
       <c r="B61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>43</v>
+      <c r="C61" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>18</v>
@@ -3346,8 +3344,8 @@
       <c r="B62" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>44</v>
+      <c r="C62" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>18</v>
@@ -3387,8 +3385,8 @@
       <c r="B63" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>45</v>
+      <c r="C63" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>12</v>
@@ -3428,8 +3426,8 @@
       <c r="B64" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>46</v>
+      <c r="C64" s="9" t="s">
+        <v>106</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>17</v>
@@ -3469,8 +3467,8 @@
       <c r="B65" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>113</v>
+      <c r="C65" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>12</v>
@@ -3510,8 +3508,8 @@
       <c r="B66" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>47</v>
+      <c r="C66" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>18</v>
@@ -3551,8 +3549,8 @@
       <c r="B67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>48</v>
+      <c r="C67" s="9" t="s">
+        <v>63</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>19</v>
@@ -3592,8 +3590,8 @@
       <c r="B68" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>49</v>
+      <c r="C68" s="9" t="s">
+        <v>108</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>17</v>
@@ -3633,8 +3631,8 @@
       <c r="B69" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>50</v>
+      <c r="C69" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>12</v>
@@ -3674,8 +3672,8 @@
       <c r="B70" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>114</v>
+      <c r="C70" s="9" t="s">
+        <v>109</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>18</v>
@@ -3715,8 +3713,8 @@
       <c r="B71" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>51</v>
+      <c r="C71" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>18</v>
@@ -3756,8 +3754,8 @@
       <c r="B72" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>52</v>
+      <c r="C72" s="9" t="s">
+        <v>110</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>17</v>
@@ -3797,8 +3795,8 @@
       <c r="B73" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>53</v>
+      <c r="C73" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>12</v>
@@ -3838,8 +3836,8 @@
       <c r="B74" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>54</v>
+      <c r="C74" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>18</v>
@@ -3879,8 +3877,8 @@
       <c r="B75" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>55</v>
+      <c r="C75" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>12</v>
@@ -3920,8 +3918,8 @@
       <c r="B76" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>56</v>
+      <c r="C76" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>12</v>
@@ -3961,8 +3959,8 @@
       <c r="B77" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>57</v>
+      <c r="C77" s="9" t="s">
+        <v>67</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
@@ -4002,8 +4000,8 @@
       <c r="B78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>115</v>
+      <c r="C78" s="9" t="s">
+        <v>113</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>12</v>
@@ -4043,8 +4041,8 @@
       <c r="B79" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>58</v>
+      <c r="C79" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>12</v>
@@ -4084,8 +4082,8 @@
       <c r="B80" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>59</v>
+      <c r="C80" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>12</v>
@@ -4125,8 +4123,8 @@
       <c r="B81" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>116</v>
+      <c r="C81" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>12</v>
@@ -4166,8 +4164,8 @@
       <c r="B82" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>60</v>
+      <c r="C82" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>12</v>
@@ -4207,8 +4205,8 @@
       <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>61</v>
+      <c r="C83" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>12</v>
@@ -4248,8 +4246,8 @@
       <c r="B84" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>62</v>
+      <c r="C84" s="9" t="s">
+        <v>116</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>12</v>
@@ -4289,8 +4287,8 @@
       <c r="B85" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>63</v>
+      <c r="C85" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>12</v>
@@ -4330,8 +4328,8 @@
       <c r="B86" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>64</v>
+      <c r="C86" s="9" t="s">
+        <v>117</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>12</v>
@@ -4368,28 +4366,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed layout, created table function, and misc.
</commit_message>
<xml_diff>
--- a/Resources/Dose Response/Information.xlsx
+++ b/Resources/Dose Response/Information.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Larz\Desktop\Thesis\Resources\Dose Response\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Larz\Desktop\Thesis\Bachelor-Thesis\Resources\Dose Response\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="117">
   <si>
     <t>1/0</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lethal </t>
   </si>
   <si>
     <t>Lethal</t>
@@ -820,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,43 +841,43 @@
   <sheetData>
     <row r="1" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -888,10 +885,10 @@
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>0</v>
@@ -923,16 +920,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -964,16 +961,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -1005,16 +1002,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -1046,16 +1043,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1087,16 +1084,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -1128,16 +1125,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -1169,16 +1166,16 @@
         <v>3</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1210,16 +1207,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
@@ -1251,16 +1248,16 @@
         <v>3</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1292,16 +1289,16 @@
         <v>3</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1333,16 +1330,16 @@
         <v>3</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1374,10 +1371,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
@@ -1415,10 +1412,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -1448,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1456,10 +1453,10 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -1489,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1497,10 +1494,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>12</v>
@@ -1530,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1538,10 +1535,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
@@ -1571,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1579,10 +1576,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
@@ -1612,7 +1609,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1620,10 +1617,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -1653,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1661,10 +1658,10 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
@@ -1694,7 +1691,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1702,10 +1699,10 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>12</v>
@@ -1735,7 +1732,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1743,10 +1740,10 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
@@ -1776,7 +1773,7 @@
         <v>1</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1784,10 +1781,10 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>12</v>
@@ -1817,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1825,10 +1822,10 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>12</v>
@@ -1858,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1866,10 +1863,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>12</v>
@@ -1899,24 +1896,24 @@
         <v>0</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1951,13 +1948,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1992,13 +1989,13 @@
         <v>6</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -2033,13 +2030,13 @@
         <v>6</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F30" s="1">
         <v>0</v>
@@ -2074,13 +2071,13 @@
         <v>6</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F31" s="1">
         <v>0</v>
@@ -2115,13 +2112,13 @@
         <v>6</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F32" s="1">
         <v>0</v>
@@ -2156,13 +2153,13 @@
         <v>6</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F33" s="1">
         <v>0</v>
@@ -2197,13 +2194,13 @@
         <v>6</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F34" s="1">
         <v>0</v>
@@ -2238,13 +2235,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -2279,7 +2276,7 @@
         <v>6</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
@@ -2309,7 +2306,7 @@
         <v>0</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2320,13 +2317,13 @@
         <v>6</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -2361,13 +2358,13 @@
         <v>6</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
@@ -2402,13 +2399,13 @@
         <v>7</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F39" s="1">
         <v>0</v>
@@ -2432,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2443,13 +2440,13 @@
         <v>7</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F40" s="1">
         <v>0</v>
@@ -2484,13 +2481,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F41" s="1">
         <v>0</v>
@@ -2525,13 +2522,13 @@
         <v>7</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
@@ -2566,13 +2563,13 @@
         <v>7</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F43" s="1">
         <v>0</v>
@@ -2607,13 +2604,13 @@
         <v>7</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F44" s="1">
         <v>0</v>
@@ -2637,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="M44" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
@@ -2648,13 +2645,13 @@
         <v>7</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F45" s="1">
         <v>0</v>
@@ -2689,13 +2686,13 @@
         <v>7</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F46" s="1">
         <v>0</v>
@@ -2730,13 +2727,13 @@
         <v>7</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F47" s="1">
         <v>0</v>
@@ -2760,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
@@ -2771,13 +2768,13 @@
         <v>7</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F48" s="1">
         <v>0</v>
@@ -2812,13 +2809,13 @@
         <v>7</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F49" s="1">
         <v>0</v>
@@ -2853,13 +2850,13 @@
         <v>7</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F50" s="1">
         <v>0</v>
@@ -2883,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -2894,13 +2891,13 @@
         <v>8</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F51" s="1">
         <v>0</v>
@@ -2924,7 +2921,7 @@
         <v>0</v>
       </c>
       <c r="M51" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -2935,13 +2932,13 @@
         <v>8</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F52" s="1">
         <v>0</v>
@@ -2965,7 +2962,7 @@
         <v>0</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -2976,13 +2973,13 @@
         <v>8</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F53" s="1">
         <v>0</v>
@@ -3006,7 +3003,7 @@
         <v>0</v>
       </c>
       <c r="M53" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -3017,13 +3014,13 @@
         <v>8</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F54" s="1">
         <v>0</v>
@@ -3047,7 +3044,7 @@
         <v>1</v>
       </c>
       <c r="M54" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -3058,13 +3055,13 @@
         <v>8</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F55" s="1">
         <v>0</v>
@@ -3088,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -3099,13 +3096,13 @@
         <v>8</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F56" s="1">
         <v>0</v>
@@ -3129,7 +3126,7 @@
         <v>1</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -3140,13 +3137,13 @@
         <v>8</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F57" s="1">
         <v>0</v>
@@ -3170,7 +3167,7 @@
         <v>1</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -3181,13 +3178,13 @@
         <v>8</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F58" s="1">
         <v>0</v>
@@ -3211,7 +3208,7 @@
         <v>0</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -3222,13 +3219,13 @@
         <v>8</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F59" s="1">
         <v>0</v>
@@ -3252,7 +3249,7 @@
         <v>1</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
@@ -3263,7 +3260,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>12</v>
@@ -3293,7 +3290,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
@@ -3304,13 +3301,13 @@
         <v>8</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F61" s="1">
         <v>0</v>
@@ -3334,7 +3331,7 @@
         <v>0</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
@@ -3345,13 +3342,13 @@
         <v>8</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F62" s="1">
         <v>0</v>
@@ -3375,7 +3372,7 @@
         <v>0</v>
       </c>
       <c r="M62" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
@@ -3386,7 +3383,7 @@
         <v>9</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>12</v>
@@ -3416,7 +3413,7 @@
         <v>1</v>
       </c>
       <c r="M63" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
@@ -3427,13 +3424,13 @@
         <v>9</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F64" s="1">
         <v>0</v>
@@ -3457,7 +3454,7 @@
         <v>1</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
@@ -3468,7 +3465,7 @@
         <v>9</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>12</v>
@@ -3498,7 +3495,7 @@
         <v>0</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
@@ -3509,13 +3506,13 @@
         <v>9</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F66" s="1">
         <v>0</v>
@@ -3539,7 +3536,7 @@
         <v>1</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
@@ -3550,10 +3547,10 @@
         <v>9</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>12</v>
@@ -3580,7 +3577,7 @@
         <v>1</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
@@ -3591,13 +3588,13 @@
         <v>9</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F68" s="1">
         <v>0</v>
@@ -3621,7 +3618,7 @@
         <v>1</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
@@ -3632,7 +3629,7 @@
         <v>9</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>12</v>
@@ -3662,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
@@ -3673,13 +3670,13 @@
         <v>9</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F70" s="1">
         <v>0</v>
@@ -3703,7 +3700,7 @@
         <v>0</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
@@ -3714,13 +3711,13 @@
         <v>9</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F71" s="1">
         <v>0</v>
@@ -3744,7 +3741,7 @@
         <v>0</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
@@ -3755,13 +3752,13 @@
         <v>9</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F72" s="1">
         <v>0</v>
@@ -3785,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -3796,7 +3793,7 @@
         <v>9</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>12</v>
@@ -3826,7 +3823,7 @@
         <v>0</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -3837,13 +3834,13 @@
         <v>9</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F74" s="1">
         <v>0</v>
@@ -3867,7 +3864,7 @@
         <v>0</v>
       </c>
       <c r="M74" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -3878,7 +3875,7 @@
         <v>10</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>12</v>
@@ -3908,7 +3905,7 @@
         <v>0</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
@@ -3919,7 +3916,7 @@
         <v>10</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>12</v>
@@ -3949,7 +3946,7 @@
         <v>0</v>
       </c>
       <c r="M76" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
@@ -3960,7 +3957,7 @@
         <v>10</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>12</v>
@@ -3990,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
@@ -4001,7 +3998,7 @@
         <v>10</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>12</v>
@@ -4031,7 +4028,7 @@
         <v>0</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.25">
@@ -4042,7 +4039,7 @@
         <v>10</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>12</v>
@@ -4072,7 +4069,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
@@ -4083,7 +4080,7 @@
         <v>10</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>12</v>
@@ -4113,7 +4110,7 @@
         <v>0</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.25">
@@ -4124,7 +4121,7 @@
         <v>10</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>12</v>
@@ -4154,7 +4151,7 @@
         <v>0</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.25">
@@ -4165,7 +4162,7 @@
         <v>10</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>12</v>
@@ -4195,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
@@ -4206,7 +4203,7 @@
         <v>10</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>12</v>
@@ -4236,7 +4233,7 @@
         <v>0</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
@@ -4247,7 +4244,7 @@
         <v>10</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>12</v>
@@ -4277,7 +4274,7 @@
         <v>0</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.25">
@@ -4288,7 +4285,7 @@
         <v>10</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>12</v>
@@ -4318,7 +4315,7 @@
         <v>0</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
@@ -4329,7 +4326,7 @@
         <v>10</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>12</v>
@@ -4359,7 +4356,7 @@
         <v>0</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>